<commit_message>
Fix jlcpcb part number
</commit_message>
<xml_diff>
--- a/schematics/m5-pantilt/jlcpcb_assembly/StackChan-BOM_JLCSMT.xlsx
+++ b/schematics/m5-pantilt/jlcpcb_assembly/StackChan-BOM_JLCSMT.xlsx
@@ -37,6 +37,7 @@
         <color rgb="FFAFABAB"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">JLCPCB Part #</t>
     </r>
@@ -46,6 +47,7 @@
         <color rgb="FFAFABAB"/>
         <rFont val="宋体"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -55,6 +57,7 @@
         <color rgb="FFAFABAB"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">optional</t>
     </r>
@@ -64,6 +67,7 @@
         <color rgb="FFAFABAB"/>
         <rFont val="宋体"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -78,7 +82,7 @@
     <t xml:space="preserve">C1206</t>
   </si>
   <si>
-    <t xml:space="preserve">C312983</t>
+    <t xml:space="preserve">C15008</t>
   </si>
   <si>
     <t xml:space="preserve">1k</t>
@@ -90,7 +94,7 @@
     <t xml:space="preserve">R0603</t>
   </si>
   <si>
-    <t xml:space="preserve">C22764</t>
+    <t xml:space="preserve">C71190</t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -114,7 +118,7 @@
     <t xml:space="preserve">R13,R14,R16</t>
   </si>
   <si>
-    <t xml:space="preserve">C23193</t>
+    <t xml:space="preserve">C21189</t>
   </si>
   <si>
     <t xml:space="preserve">R2</t>
@@ -205,6 +209,7 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -227,24 +232,28 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFAFABAB"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFAFABAB"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,12 +340,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -402,22 +411,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>